<commit_message>
Write a new dFBA simulator, add DHPS reactions
</commit_message>
<xml_diff>
--- a/data/drawdown_raw.xlsx
+++ b/data/drawdown_raw.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a30fe02b4181869d/SchoolWork/Stanford Grad/Projects/Covert Lab/Oceans/rpom-fba/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{FA0EDAC4-1605-4766-880F-60C5133F8F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7373182-9685-4956-B28B-F7CB861ACA09}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{FA0EDAC4-1605-4766-880F-60C5133F8F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09169258-D317-4262-B616-862D0798FE05}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1350" windowWidth="15980" windowHeight="9330" activeTab="1" xr2:uid="{E2B09790-CECF-4BB6-A879-ED32A985B05F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E2B09790-CECF-4BB6-A879-ED32A985B05F}"/>
   </bookViews>
   <sheets>
     <sheet name="drawdown_clean" sheetId="2" r:id="rId1"/>
@@ -206,10 +206,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -501,7 +497,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -515,13 +511,13 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -532,7 +528,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -543,7 +539,7 @@
         <v>82.430213690000002</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -554,7 +550,7 @@
         <v>85.087625930000002</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -565,7 +561,7 @@
         <v>42.515250760000001</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -576,7 +572,7 @@
         <v>53.408536949999998</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -587,7 +583,7 @@
         <v>45.977560660000002</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -598,7 +594,7 @@
         <v>24.048474720000002</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -609,7 +605,7 @@
         <v>19.945106200000001</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -620,7 +616,7 @@
         <v>8.7443750490000003</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -631,7 +627,7 @@
         <v>10.22232545</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -642,7 +638,7 @@
         <v>10.56628173</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -653,7 +649,7 @@
         <v>9.8917357280000004</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -664,7 +660,7 @@
         <v>7.1186285829999996</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -675,7 +671,7 @@
         <v>3.9746389039999999</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -686,7 +682,7 @@
         <v>5.5749585980000003</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -697,7 +693,7 @@
         <v>5.6658924969999998</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -708,7 +704,7 @@
         <v>114.9081175</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -719,7 +715,7 @@
         <v>106.6768962</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -730,7 +726,7 @@
         <v>80.943227309999997</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -741,7 +737,7 @@
         <v>82.90748121</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -752,7 +748,7 @@
         <v>96.986355110000005</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -763,7 +759,7 @@
         <v>142.84040899999999</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -774,7 +770,7 @@
         <v>93.671471530000005</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -785,7 +781,7 @@
         <v>20.677636490000001</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -796,7 +792,7 @@
         <v>18.990885089999999</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -807,7 +803,7 @@
         <v>19.718534460000001</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -818,7 +814,7 @@
         <v>165.5112201</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -829,7 +825,7 @@
         <v>168.40114220000001</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -840,7 +836,7 @@
         <v>7.2679684999999994E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -851,7 +847,7 @@
         <v>6.5802806790000004</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -862,7 +858,7 @@
         <v>3.076779583</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -873,7 +869,7 @@
         <v>190.97237269999999</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -884,7 +880,7 @@
         <v>138.99128920000001</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>13</v>
       </c>
@@ -895,7 +891,7 @@
         <v>8.7483738950000003</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -906,7 +902,7 @@
         <v>12.28836499</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -917,7 +913,7 @@
         <v>6.8100903849999996</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -928,7 +924,7 @@
         <v>83.989698599999997</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -939,7 +935,7 @@
         <v>87.830573270000002</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -950,7 +946,7 @@
         <v>0.39286617200000001</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -961,7 +957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -972,7 +968,7 @@
         <v>0.56160657700000005</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>18</v>
       </c>
@@ -983,7 +979,7 @@
         <v>8.2062793999999994E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>18</v>
       </c>
@@ -994,7 +990,7 @@
         <v>9.8581716999999999E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>18</v>
       </c>
@@ -1005,7 +1001,7 @@
         <v>8.6924009999999996E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>18</v>
       </c>
@@ -1016,7 +1012,7 @@
         <v>1.2782922459999999</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>18</v>
       </c>
@@ -1027,7 +1023,7 @@
         <v>1.079225608</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -1038,7 +1034,7 @@
         <v>10.400156539999999</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -1049,7 +1045,7 @@
         <v>9.99192635</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>8</v>
       </c>
@@ -1060,7 +1056,7 @@
         <v>0.35943340200000001</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>8</v>
       </c>
@@ -1071,7 +1067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -1082,7 +1078,7 @@
         <v>0.55178091100000004</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>17</v>
       </c>
@@ -1093,7 +1089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>17</v>
       </c>
@@ -1104,7 +1100,7 @@
         <v>0.336566278</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>17</v>
       </c>
@@ -1115,7 +1111,7 @@
         <v>0.30489519799999998</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>17</v>
       </c>
@@ -1126,7 +1122,7 @@
         <v>44.017821400000003</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>17</v>
       </c>
@@ -1137,7 +1133,7 @@
         <v>79.840110280000005</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>19</v>
       </c>
@@ -1148,7 +1144,7 @@
         <v>58.617029459999998</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>19</v>
       </c>
@@ -1159,7 +1155,7 @@
         <v>64.689339599999997</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>19</v>
       </c>
@@ -1170,7 +1166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>19</v>
       </c>
@@ -1181,7 +1177,7 @@
         <v>0.45621520300000001</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>19</v>
       </c>
@@ -1192,7 +1188,7 @@
         <v>0.81466164699999999</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>20</v>
       </c>
@@ -1203,7 +1199,7 @@
         <v>0.28006355900000002</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>20</v>
       </c>
@@ -1214,7 +1210,7 @@
         <v>0.39502720000000002</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>20</v>
       </c>
@@ -1225,7 +1221,7 @@
         <v>0.45088361799999999</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>20</v>
       </c>
@@ -1236,7 +1232,7 @@
         <v>104.8657451</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>20</v>
       </c>
@@ -1247,7 +1243,7 @@
         <v>106.07019990000001</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>2</v>
       </c>
@@ -1258,7 +1254,7 @@
         <v>0.28725089999999998</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>2</v>
       </c>
@@ -1269,7 +1265,7 @@
         <v>0.26021685999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>2</v>
       </c>
@@ -1280,7 +1276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>2</v>
       </c>
@@ -1291,7 +1287,7 @@
         <v>133.8236967</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>2</v>
       </c>
@@ -1302,7 +1298,7 @@
         <v>138.8920382</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>21</v>
       </c>
@@ -1313,7 +1309,7 @@
         <v>55.934828779999997</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>21</v>
       </c>
@@ -1324,7 +1320,7 @@
         <v>73.768810529999996</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>21</v>
       </c>
@@ -1335,7 +1331,7 @@
         <v>69.553757439999998</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>21</v>
       </c>
@@ -1346,7 +1342,7 @@
         <v>117.29532570000001</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>21</v>
       </c>
@@ -1357,7 +1353,7 @@
         <v>116.11653269999999</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>24</v>
       </c>
@@ -1368,7 +1364,7 @@
         <v>18.406889379999999</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>24</v>
       </c>
@@ -1379,7 +1375,7 @@
         <v>16.661911809999999</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>24</v>
       </c>
@@ -1390,7 +1386,7 @@
         <v>11.315315610000001</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>24</v>
       </c>
@@ -1401,7 +1397,7 @@
         <v>12.126346789999999</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>24</v>
       </c>
@@ -1412,7 +1408,7 @@
         <v>13.0735513</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>23</v>
       </c>
@@ -1423,7 +1419,7 @@
         <v>72.548742779999998</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>23</v>
       </c>
@@ -1434,7 +1430,7 @@
         <v>73.094444280000005</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>23</v>
       </c>
@@ -1445,7 +1441,7 @@
         <v>8.4761317930000004</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>23</v>
       </c>
@@ -1456,7 +1452,7 @@
         <v>1.3779288709999999</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>23</v>
       </c>
@@ -1467,7 +1463,7 @@
         <v>7.6725253010000003</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>22</v>
       </c>
@@ -1478,7 +1474,7 @@
         <v>237.43492140000001</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>22</v>
       </c>
@@ -1489,7 +1485,7 @@
         <v>220.95530479999999</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>22</v>
       </c>
@@ -1500,7 +1496,7 @@
         <v>132.44767830000001</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>22</v>
       </c>
@@ -1511,7 +1507,7 @@
         <v>131.12463589999999</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>22</v>
       </c>
@@ -1522,7 +1518,7 @@
         <v>149.6756226</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>5</v>
       </c>
@@ -1533,7 +1529,7 @@
         <v>88.324231150000003</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>5</v>
       </c>
@@ -1544,7 +1540,7 @@
         <v>85.352866550000002</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>5</v>
       </c>
@@ -1555,7 +1551,7 @@
         <v>52.925675290000001</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>5</v>
       </c>
@@ -1566,7 +1562,7 @@
         <v>52.816251899999997</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>5</v>
       </c>
@@ -1577,7 +1573,7 @@
         <v>52.275496459999999</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>26</v>
       </c>
@@ -1588,7 +1584,7 @@
         <v>0.69115781499999995</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>26</v>
       </c>
@@ -1599,7 +1595,7 @@
         <v>0.12357362099999999</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>26</v>
       </c>
@@ -1610,7 +1606,7 @@
         <v>2.9889397000000002E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>26</v>
       </c>
@@ -1621,7 +1617,7 @@
         <v>41.572808719999998</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>26</v>
       </c>
@@ -1632,7 +1628,7 @@
         <v>38.86885315</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>25</v>
       </c>
@@ -1643,7 +1639,7 @@
         <v>285.54860830000001</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>25</v>
       </c>
@@ -1654,7 +1650,7 @@
         <v>270.09685339999999</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>25</v>
       </c>
@@ -1665,7 +1661,7 @@
         <v>83.070779389999998</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>25</v>
       </c>
@@ -1676,7 +1672,7 @@
         <v>87.012967750000001</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>25</v>
       </c>
@@ -1698,20 +1694,20 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1731,7 +1727,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1749,7 +1745,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1767,7 +1763,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1785,7 +1781,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1803,7 +1799,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1821,7 +1817,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1839,7 +1835,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1857,7 +1853,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1875,7 +1871,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1896,7 +1892,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1914,7 +1910,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1935,7 +1931,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1953,7 +1949,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1971,7 +1967,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1989,7 +1985,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -2007,7 +2003,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -2025,7 +2021,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -2046,7 +2042,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -2064,7 +2060,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -2082,7 +2078,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -2103,7 +2099,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>

</xml_diff>